<commit_message>
Actualización del Back 2025-07-09
</commit_message>
<xml_diff>
--- a/senosiain/Alta Trabajadores/Layout alta Trabajadores Adam.xlsx
+++ b/senosiain/Alta Trabajadores/Layout alta Trabajadores Adam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Terceros\fortia\senosiain\Alta Trabajadores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Terceros\fortia\Senosiain\Alta Trabajadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B8AE81-0634-4092-94E9-5A1DF582D192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D10C65-A24B-438B-9127-5D20D7FB7563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{97D2984B-2E06-40FC-8099-9ADEE5747D5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="13" xr2:uid="{97D2984B-2E06-40FC-8099-9ADEE5747D5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Trabajadores" sheetId="2" r:id="rId1"/>
@@ -1126,14 +1126,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2544,7 +2544,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -3032,8 +3032,8 @@
   <sheetPr codeName="Hoja13"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3247,7 +3247,7 @@
   <sheetPr codeName="Hoja11"/>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -3784,11 +3784,11 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.4">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3807,7 +3807,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3931,8 +3931,8 @@
   <sheetPr codeName="Hoja14"/>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4116,24 +4116,24 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4714,14 +4714,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.4">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4882,8 +4882,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4968,7 +4968,7 @@
       <c r="C8" s="2">
         <v>10</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="36" t="s">
         <v>118</v>
       </c>
       <c r="E8" s="2"/>
@@ -5136,7 +5136,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5548,7 +5548,9 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Actualización Procedimientos de Pensiones
</commit_message>
<xml_diff>
--- a/senosiain/Alta Trabajadores/Layout alta Trabajadores Adam.xlsx
+++ b/senosiain/Alta Trabajadores/Layout alta Trabajadores Adam.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Terceros\fortia\Senosiain\Alta Trabajadores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D10C65-A24B-438B-9127-5D20D7FB7563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED9008-B01C-45B1-8EC7-4584462C8F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="13" xr2:uid="{97D2984B-2E06-40FC-8099-9ADEE5747D5D}"/>
   </bookViews>
@@ -2544,7 +2544,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -3248,7 +3248,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>